<commit_message>
added a new pool
</commit_message>
<xml_diff>
--- a/ Hacktoberfest_database.xlsx
+++ b/ Hacktoberfest_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshul.choudhary@ibm.com/PycharmProjects/Manipulating_Excel_Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19031311-B79F-DF4C-95DA-C47EAF9E3CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6867BB8-9BF1-3B49-9383-CFCFC74C3B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31040" yWindow="460" windowWidth="30880" windowHeight="28200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="460" windowWidth="30880" windowHeight="26800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heading 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>YELLOW</t>
   </si>
@@ -35,30 +35,12 @@
     <t>BLUE</t>
   </si>
   <si>
-    <t>/Users/anshul.choudhary@ibm.com/PycharmProjects/Auto-Opsi/demo8.xlsx</t>
-  </si>
-  <si>
-    <t>1.2.3.0/24</t>
-  </si>
-  <si>
     <t>PRESUME ALL OTHER 1x ARE BLUE</t>
   </si>
   <si>
     <t>(EXCLUDING 1.2.0.0/16)</t>
   </si>
   <si>
-    <t>1.2.6.0/24</t>
-  </si>
-  <si>
-    <t>1.2.41.0/24</t>
-  </si>
-  <si>
-    <t>1.2.42.0/23</t>
-  </si>
-  <si>
-    <t>1.2.10.0/23</t>
-  </si>
-  <si>
     <t>1.2.11.0/24</t>
   </si>
   <si>
@@ -86,14 +68,143 @@
     <t>Ip outside 1x are all red</t>
   </si>
   <si>
-    <t>http://jodies.de/ipcalc</t>
+    <t xml:space="preserve">1.2.4.0/23    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.14.0/23   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.13.0/24   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.16.0/21   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.24.0/22   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.28.0/24   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.29.0/25   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.29.128/25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.41.128/26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.41.192/26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.92.0/23   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.91.0/24   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.94.0/24   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.95.128/26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.95.192/26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.96.0/21   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.104.0/22  </t>
+  </si>
+  <si>
+    <t>1.2.108.128/25</t>
+  </si>
+  <si>
+    <t>1.2.89.0/24</t>
+  </si>
+  <si>
+    <t>1.2.90.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.44.64/26  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.44.0/27   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.44.32/27  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.44.128/27 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.120.0/23  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.122.0/27  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.122.32/27 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.122.64/27 </t>
+  </si>
+  <si>
+    <t>1.2.170.0/23</t>
+  </si>
+  <si>
+    <t>1.2.172.0/27</t>
+  </si>
+  <si>
+    <t>1.2.172.32/27</t>
+  </si>
+  <si>
+    <t>1.2.172.128/27</t>
+  </si>
+  <si>
+    <t>1.2.142.0/23</t>
+  </si>
+  <si>
+    <t>1.2.141.0/24</t>
+  </si>
+  <si>
+    <t>1.2.144.0/21</t>
+  </si>
+  <si>
+    <t>1.2.152.0/22</t>
+  </si>
+  <si>
+    <t>1.2.156.0/24</t>
+  </si>
+  <si>
+    <t>1.2.157.0/25</t>
+  </si>
+  <si>
+    <t>1.2.157.128/25</t>
+  </si>
+  <si>
+    <t>1.2.169.0/26</t>
+  </si>
+  <si>
+    <t>1.2.169.64/26</t>
+  </si>
+  <si>
+    <t>1.2.139.0/24</t>
+  </si>
+  <si>
+    <t>1.2.140.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.108.0/25  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,14 +223,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,9 +275,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -184,15 +286,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,40 +609,40 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="33.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -549,155 +650,208 @@
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C7" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="C11" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8"/>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9"/>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10"/>
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11"/>
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12"/>
-      <c r="C12"/>
+      <c r="C12" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13"/>
+      <c r="B13" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14"/>
+      <c r="B14" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15"/>
+      <c r="B15" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16"/>
+      <c r="B16" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17"/>
+      <c r="B17" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18"/>
+      <c r="B18" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19"/>
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20"/>
+      <c r="B20" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21"/>
+      <c r="B21" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22"/>
+      <c r="B22" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23"/>
+      <c r="B23" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24"/>
+      <c r="B24" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" xr:uid="{2A45D26F-C550-A74E-80DE-3D07A858080C}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="8" customWidth="1"/>
     <col min="4" max="4" width="30.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -705,72 +859,84 @@
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>4</v>
+      <c r="B12" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A44" r:id="rId1" xr:uid="{49470ECE-EC36-A743-8432-1BE9AE33C821}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>